<commit_message>
update on time series models
</commit_message>
<xml_diff>
--- a/MAPE Comparision for Models.xlsx
+++ b/MAPE Comparision for Models.xlsx
@@ -9,12 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24480" windowHeight="16260" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Prediction of Load" sheetId="1" r:id="rId1"/>
     <sheet name="Prediction of Peakhour" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet1!$F$7:$H$23</definedName>
+  </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -28,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="26">
   <si>
     <t>naive_model</t>
   </si>
@@ -67,13 +71,52 @@
   </si>
   <si>
     <t>HoltWinters_expo_model</t>
+  </si>
+  <si>
+    <t>Prediction of Peakhour</t>
+  </si>
+  <si>
+    <t>Prediction of Load</t>
+  </si>
+  <si>
+    <t>Train</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>theta</t>
+  </si>
+  <si>
+    <t>ets_model</t>
+  </si>
+  <si>
+    <t>arima_fourier_model</t>
+  </si>
+  <si>
+    <t>theta_model</t>
+  </si>
+  <si>
+    <t>HoltWinters with Additive Seasonality model</t>
+  </si>
+  <si>
+    <t>Prediction of Daily Peak hour</t>
+  </si>
+  <si>
+    <t>Prediction for 2005 Load</t>
+  </si>
+  <si>
+    <t>Prediction for Peak hour</t>
+  </si>
+  <si>
+    <t>Arima Fourier Model</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -97,8 +140,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -111,8 +176,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5B9BD5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBDD6EE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDEEAF6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -120,23 +203,232 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="65">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -415,7 +707,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15:R17"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -480,7 +772,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>17.728300000000001</v>
@@ -518,7 +810,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>16.380520000000001</v>
@@ -556,10 +848,10 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -692,13 +984,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="8" max="8" width="39.6640625" customWidth="1"/>
+    <col min="9" max="9" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -738,7 +1032,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>24.92822</v>
@@ -776,7 +1070,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>17.470120000000001</v>
@@ -812,12 +1106,23 @@
         <v>20.620650000000001</v>
       </c>
     </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -830,6 +1135,9 @@
       <c r="C12">
         <v>17.470120000000001</v>
       </c>
+      <c r="G12" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -944,4 +1252,640 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="46.1640625" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="4" max="5" width="20.6640625" customWidth="1"/>
+    <col min="6" max="6" width="34.5" customWidth="1"/>
+    <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>24.92822</v>
+      </c>
+      <c r="C2">
+        <v>30.019130000000001</v>
+      </c>
+      <c r="D2">
+        <v>22.49907</v>
+      </c>
+      <c r="E2">
+        <v>15.94201</v>
+      </c>
+      <c r="F2">
+        <v>25.056470000000001</v>
+      </c>
+      <c r="G2">
+        <v>17.515799999999999</v>
+      </c>
+      <c r="H2">
+        <v>23.28754</v>
+      </c>
+      <c r="I2">
+        <v>23.289470000000001</v>
+      </c>
+      <c r="J2">
+        <v>18.311409999999999</v>
+      </c>
+      <c r="K2">
+        <v>18.32123</v>
+      </c>
+      <c r="L2">
+        <v>23.405370000000001</v>
+      </c>
+      <c r="M2">
+        <v>18.360060000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>17.470120000000001</v>
+      </c>
+      <c r="C3">
+        <v>20.03753</v>
+      </c>
+      <c r="D3">
+        <v>20.395250000000001</v>
+      </c>
+      <c r="E3">
+        <v>16.69605</v>
+      </c>
+      <c r="F3">
+        <v>18.161259999999999</v>
+      </c>
+      <c r="G3">
+        <v>16.880610000000001</v>
+      </c>
+      <c r="H3">
+        <v>16.910979999999999</v>
+      </c>
+      <c r="I3">
+        <v>17.094390000000001</v>
+      </c>
+      <c r="J3">
+        <v>16.57884</v>
+      </c>
+      <c r="K3">
+        <v>16.62039</v>
+      </c>
+      <c r="L3">
+        <v>20.620650000000001</v>
+      </c>
+      <c r="M3">
+        <v>16.527159999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="H8" s="2"/>
+      <c r="N8" t="s">
+        <v>11</v>
+      </c>
+      <c r="O8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M9" t="s">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>17.728300000000001</v>
+      </c>
+      <c r="O9">
+        <v>16.380520000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>2.14995</v>
+      </c>
+      <c r="C10">
+        <v>15.40401</v>
+      </c>
+      <c r="D10" s="1">
+        <v>18.360060000000001</v>
+      </c>
+      <c r="E10" s="1">
+        <v>16.527159999999999</v>
+      </c>
+      <c r="M10" t="s">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>3.1206369999999999</v>
+      </c>
+      <c r="O10">
+        <v>27.010643999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>2.5012629999999998</v>
+      </c>
+      <c r="C11">
+        <v>18.033887</v>
+      </c>
+      <c r="D11">
+        <v>18.311409999999999</v>
+      </c>
+      <c r="E11">
+        <v>16.57884</v>
+      </c>
+      <c r="M11" t="s">
+        <v>2</v>
+      </c>
+      <c r="N11">
+        <v>2.4823460000000002</v>
+      </c>
+      <c r="O11">
+        <v>25.363990000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>2.3442050000000001</v>
+      </c>
+      <c r="C12">
+        <v>18.287523</v>
+      </c>
+      <c r="D12">
+        <v>18.32123</v>
+      </c>
+      <c r="E12">
+        <v>16.62039</v>
+      </c>
+      <c r="M12" t="s">
+        <v>3</v>
+      </c>
+      <c r="N12">
+        <v>0.98617200000000005</v>
+      </c>
+      <c r="O12">
+        <v>16.324152000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>0.98617200000000005</v>
+      </c>
+      <c r="C13">
+        <v>16.324152000000002</v>
+      </c>
+      <c r="D13">
+        <v>15.94201</v>
+      </c>
+      <c r="E13">
+        <v>16.69605</v>
+      </c>
+      <c r="M13" t="s">
+        <v>4</v>
+      </c>
+      <c r="N13">
+        <v>20.70072</v>
+      </c>
+      <c r="O13">
+        <v>22.426780000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>1.206612</v>
+      </c>
+      <c r="C14">
+        <v>15.193803000000001</v>
+      </c>
+      <c r="D14">
+        <v>17.515799999999999</v>
+      </c>
+      <c r="E14">
+        <v>16.880610000000001</v>
+      </c>
+      <c r="M14" t="s">
+        <v>5</v>
+      </c>
+      <c r="N14">
+        <v>1.206612</v>
+      </c>
+      <c r="O14">
+        <v>15.193803000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15">
+        <v>2.1517390000000001</v>
+      </c>
+      <c r="C15">
+        <v>15.202197999999999</v>
+      </c>
+      <c r="D15">
+        <v>23.28754</v>
+      </c>
+      <c r="E15">
+        <v>16.910979999999999</v>
+      </c>
+      <c r="M15" t="s">
+        <v>6</v>
+      </c>
+      <c r="N15">
+        <v>2.1517390000000001</v>
+      </c>
+      <c r="O15">
+        <v>15.202197999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <v>2.1517059999999999</v>
+      </c>
+      <c r="C16">
+        <v>15.518230000000001</v>
+      </c>
+      <c r="D16">
+        <v>23.289470000000001</v>
+      </c>
+      <c r="E16">
+        <v>17.094390000000001</v>
+      </c>
+      <c r="M16" t="s">
+        <v>7</v>
+      </c>
+      <c r="N16">
+        <v>2.1517059999999999</v>
+      </c>
+      <c r="O16">
+        <v>15.518230000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>17.728300000000001</v>
+      </c>
+      <c r="C17">
+        <v>16.380520000000001</v>
+      </c>
+      <c r="D17">
+        <v>24.92822</v>
+      </c>
+      <c r="E17">
+        <v>17.470120000000001</v>
+      </c>
+      <c r="M17" t="s">
+        <v>8</v>
+      </c>
+      <c r="N17">
+        <v>2.5012629999999998</v>
+      </c>
+      <c r="O17">
+        <v>18.033887</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>20.70072</v>
+      </c>
+      <c r="C18">
+        <v>22.426780000000001</v>
+      </c>
+      <c r="D18">
+        <v>25.056470000000001</v>
+      </c>
+      <c r="E18">
+        <v>18.161259999999999</v>
+      </c>
+      <c r="M18" t="s">
+        <v>9</v>
+      </c>
+      <c r="N18">
+        <v>2.3442050000000001</v>
+      </c>
+      <c r="O18">
+        <v>18.287523</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>3.1206369999999999</v>
+      </c>
+      <c r="C19">
+        <v>27.010643999999999</v>
+      </c>
+      <c r="D19">
+        <v>30.019130000000001</v>
+      </c>
+      <c r="E19">
+        <v>20.03753</v>
+      </c>
+      <c r="M19" t="s">
+        <v>12</v>
+      </c>
+      <c r="N19">
+        <v>7.0784710000000004</v>
+      </c>
+      <c r="O19">
+        <v>29.019098</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>2.4823460000000002</v>
+      </c>
+      <c r="C20">
+        <v>25.363990000000001</v>
+      </c>
+      <c r="D20">
+        <v>22.49907</v>
+      </c>
+      <c r="E20">
+        <v>20.395250000000001</v>
+      </c>
+      <c r="M20" t="s">
+        <v>18</v>
+      </c>
+      <c r="N20">
+        <v>3.836214</v>
+      </c>
+      <c r="O20">
+        <v>36.599170000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21">
+        <v>7.0784710000000004</v>
+      </c>
+      <c r="C21">
+        <v>29.019098</v>
+      </c>
+      <c r="D21">
+        <v>23.405370000000001</v>
+      </c>
+      <c r="E21">
+        <v>20.620650000000001</v>
+      </c>
+      <c r="M21" t="s">
+        <v>19</v>
+      </c>
+      <c r="N21">
+        <v>4.682404</v>
+      </c>
+      <c r="O21">
+        <v>17.13954</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>3.836214</v>
+      </c>
+      <c r="C22">
+        <v>36.599170000000001</v>
+      </c>
+      <c r="M22" t="s">
+        <v>20</v>
+      </c>
+      <c r="N22">
+        <v>2.14995</v>
+      </c>
+      <c r="O22">
+        <v>15.40401</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23">
+        <v>4.682404</v>
+      </c>
+      <c r="C23">
+        <v>17.13954</v>
+      </c>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="5">
+        <v>2.14995</v>
+      </c>
+      <c r="C30" s="5">
+        <v>18.360060000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="5">
+        <v>15.40401</v>
+      </c>
+      <c r="C31" s="5">
+        <v>16.527159999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="10">
+        <v>4.682404</v>
+      </c>
+      <c r="C34" s="10"/>
+    </row>
+    <row r="35" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="11">
+        <v>17.13954</v>
+      </c>
+      <c r="C35" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D7:E8"/>
+    <mergeCell ref="B7:C8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>